<commit_message>
fix table error and more
</commit_message>
<xml_diff>
--- a/relationship.xlsx
+++ b/relationship.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mark\Documents\Mark\Project\20210606 Dynamic Relationship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B7A32D6-A83F-4CE2-A630-25DA367E4C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3409CD98-D620-49A5-B573-776CF4F546BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="6300" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{C0A86CE9-5774-486B-821C-E24FED4D1238}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C0A86CE9-5774-486B-821C-E24FED4D1238}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="relationship" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="20">
   <si>
     <t>Terran</t>
   </si>
@@ -80,6 +81,12 @@
   </si>
   <si>
     <t>Main+Copr-Dukes</t>
+  </si>
+  <si>
+    <t>Boron</t>
+  </si>
+  <si>
+    <t>TerraCorp</t>
   </si>
 </sst>
 </file>
@@ -441,7 +448,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="A1:P16"/>
+      <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,6 +710,9 @@
       <c r="C6">
         <v>-0.3</v>
       </c>
+      <c r="D6">
+        <v>-0.3</v>
+      </c>
       <c r="E6">
         <v>-0.3</v>
       </c>
@@ -729,15 +739,15 @@
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>-0.89999999999999991</v>
+        <v>-1.2</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>-1.6500000000000001</v>
+        <v>-1.9500000000000002</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>-1.8</v>
+        <v>-2.1</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -838,6 +848,9 @@
       <c r="I9">
         <v>1</v>
       </c>
+      <c r="J9">
+        <v>-0.3</v>
+      </c>
       <c r="K9">
         <v>-0.3</v>
       </c>
@@ -873,6 +886,9 @@
       <c r="C10">
         <v>-0.3</v>
       </c>
+      <c r="D10">
+        <v>-0.15</v>
+      </c>
       <c r="E10">
         <v>-0.3</v>
       </c>
@@ -883,6 +899,9 @@
         <v>-0.3</v>
       </c>
       <c r="H10">
+        <v>-0.3</v>
+      </c>
+      <c r="I10">
         <v>-0.3</v>
       </c>
       <c r="J10">
@@ -902,15 +921,15 @@
       </c>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>-1.5</v>
+        <v>-1.6500000000000001</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>-2.6999999999999997</v>
+        <v>-2.8499999999999996</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>-2.4</v>
+        <v>-2.5499999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1023,6 +1042,9 @@
       <c r="C13">
         <v>-0.3</v>
       </c>
+      <c r="D13">
+        <v>-0.3</v>
+      </c>
       <c r="E13">
         <v>-0.3</v>
       </c>
@@ -1046,15 +1068,15 @@
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>-1.5</v>
+        <v>-1.8</v>
       </c>
       <c r="S13" s="1">
         <f t="shared" si="1"/>
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="T13">
         <f t="shared" si="2"/>
-        <v>-1.5</v>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1093,6 +1115,9 @@
       <c r="C15">
         <v>-0.3</v>
       </c>
+      <c r="D15">
+        <v>-0.3</v>
+      </c>
       <c r="E15">
         <v>0.05</v>
       </c>
@@ -1116,15 +1141,15 @@
       </c>
       <c r="R15">
         <f t="shared" si="0"/>
-        <v>-0.24999999999999997</v>
+        <v>-0.54999999999999993</v>
       </c>
       <c r="S15" s="1">
         <f t="shared" si="1"/>
-        <v>0.15000000000000005</v>
+        <v>-0.15</v>
       </c>
       <c r="T15" s="1">
         <f t="shared" si="2"/>
-        <v>0.15000000000000005</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1137,6 +1162,9 @@
       <c r="C16">
         <v>0.05</v>
       </c>
+      <c r="D16">
+        <v>0.15</v>
+      </c>
       <c r="E16">
         <v>-0.3</v>
       </c>
@@ -1163,15 +1191,15 @@
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
-        <v>-0.24999999999999997</v>
+        <v>-0.1</v>
       </c>
       <c r="S16" s="1">
         <f t="shared" si="1"/>
-        <v>0.35000000000000009</v>
+        <v>0.5</v>
       </c>
       <c r="T16" s="1">
         <f t="shared" si="2"/>
-        <v>0.35000000000000009</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1192,36 +1220,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A5EF90-5B9D-445C-A341-B1DC8077A761}">
-  <dimension ref="A1:Q16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B217405C-BB9F-4C27-BAAA-396785726FB7}">
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>10</v>
@@ -1249,14 +1277,14 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1268,10 +1296,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1295,25 +1323,25 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="Q2">
         <f>SUM(B2:P2)</f>
-        <v>1.1000000000000001</v>
+        <v>0.84999999999999987</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1337,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1349,37 +1377,37 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q16" si="0">SUM(B3:P3)</f>
+        <f>SUM(B3:P3)</f>
         <v>0.84999999999999987</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1391,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1406,13 +1434,13 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
-        <v>0.84999999999999987</v>
+        <f>SUM(B4:P4)</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1421,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1430,43 +1458,43 @@
         <v>-0.15</v>
       </c>
       <c r="G5">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
       <c r="H5">
-        <v>-0.3</v>
+        <v>0.05</v>
       </c>
       <c r="I5">
-        <v>0.15</v>
+        <v>-0.15</v>
       </c>
       <c r="J5">
-        <v>-0.3</v>
+        <v>0.05</v>
       </c>
       <c r="K5">
-        <v>-0.15</v>
+        <v>-0.3</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0.05</v>
+        <v>-0.3</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="O5">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
-        <v>-0.15000000000000002</v>
+        <f>SUM(B5:P5)</f>
+        <v>-9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1475,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="E6">
         <v>-0.15</v>
@@ -1484,38 +1512,38 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.15</v>
+        <v>-0.15</v>
       </c>
       <c r="H6">
-        <v>0.05</v>
+        <v>-0.3</v>
       </c>
       <c r="I6">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
       <c r="J6">
-        <v>0.05</v>
+        <v>-0.3</v>
       </c>
       <c r="K6">
-        <v>-0.3</v>
+        <v>-0.15</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>-0.3</v>
+        <v>0.05</v>
       </c>
       <c r="N6">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="P6">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
-        <v>-0.24999999999999983</v>
+        <f>SUM(B6:P6)</f>
+        <v>-0.44999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1523,19 +1551,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E7">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
       <c r="F7">
-        <v>0.15</v>
+        <v>-0.15</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1568,28 +1596,28 @@
         <v>-0.3</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f>SUM(B7:P7)</f>
         <v>-0.25000000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E8">
-        <v>-0.3</v>
+        <v>0.05</v>
       </c>
       <c r="F8">
-        <v>0.05</v>
+        <v>-0.3</v>
       </c>
       <c r="G8">
         <v>0.15</v>
@@ -1622,7 +1650,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
+        <f>SUM(B8:P8)</f>
         <v>-0.49999999999999994</v>
       </c>
     </row>
@@ -1640,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.15</v>
+        <v>-0.15</v>
       </c>
       <c r="F9">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
       <c r="G9">
         <v>-0.15</v>
@@ -1658,7 +1686,7 @@
         <v>-0.3</v>
       </c>
       <c r="K9">
-        <v>0.15</v>
+        <v>-0.15</v>
       </c>
       <c r="L9">
         <v>-0.3</v>
@@ -1676,8 +1704,8 @@
         <v>-0.3</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="0"/>
-        <v>-0.35</v>
+        <f>SUM(B9:P9)</f>
+        <v>-0.64999999999999991</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1694,10 +1722,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>-0.3</v>
+        <v>0.05</v>
       </c>
       <c r="F10">
-        <v>0.05</v>
+        <v>-0.3</v>
       </c>
       <c r="G10">
         <v>0.05</v>
@@ -1730,7 +1758,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f>SUM(B10:P10)</f>
         <v>-0.7</v>
       </c>
     </row>
@@ -1748,10 +1776,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>-0.15</v>
+        <v>-0.3</v>
       </c>
       <c r="F11">
-        <v>-0.3</v>
+        <v>-0.15</v>
       </c>
       <c r="G11">
         <v>0.15</v>
@@ -1760,7 +1788,7 @@
         <v>0.05</v>
       </c>
       <c r="I11">
-        <v>0.15</v>
+        <v>-0.15</v>
       </c>
       <c r="J11">
         <v>-0.3</v>
@@ -1784,8 +1812,8 @@
         <v>-0.3</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="0"/>
-        <v>-0.59999999999999987</v>
+        <f>SUM(B11:P11)</f>
+        <v>-0.89999999999999991</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1796,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="D12">
         <v>-0.3</v>
@@ -1838,8 +1866,8 @@
         <v>-0.3</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
-        <v>-0.95</v>
+        <f>SUM(B12:P12)</f>
+        <v>-1.25</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1856,10 +1884,10 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
+        <v>-0.3</v>
       </c>
       <c r="F13">
-        <v>-0.3</v>
+        <v>0.05</v>
       </c>
       <c r="G13">
         <v>-0.3</v>
@@ -1892,7 +1920,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="0"/>
+        <f>SUM(B13:P13)</f>
         <v>-1.2000000000000002</v>
       </c>
     </row>
@@ -1907,13 +1935,13 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="F14">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>-0.3</v>
@@ -1946,8 +1974,8 @@
         <v>-0.3</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="0"/>
-        <v>-1.2500000000000002</v>
+        <f>SUM(B14:P14)</f>
+        <v>-1.5500000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1964,10 +1992,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="G15">
         <v>-0.3</v>
@@ -1997,11 +2025,11 @@
         <v>1</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="0"/>
-        <v>-1.6999999999999997</v>
+        <f>SUM(B15:P15)</f>
+        <v>-1.9999999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -2009,19 +2037,19 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="C16">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="F16">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>-0.3</v>
@@ -2048,32 +2076,86 @@
         <v>-0.3</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="P16">
         <v>1</v>
       </c>
       <c r="Q16">
+        <f>SUM(B16:P16)</f>
+        <v>-2.4499999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>SUM(B2:B16)</f>
+        <v>0.84999999999999987</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:P17" si="0">SUM(C2:C16)</f>
+        <v>0.84999999999999987</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
-        <v>-1.9999999999999996</v>
+        <v>0.19999999999999993</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>-9.9999999999999978E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>-0.25000000000000006</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>-0.49999999999999994</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>-0.64999999999999991</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>-0.7</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>-0.95</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>-1.2000000000000002</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>-1.2500000000000002</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>-1.9999999999999998</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>-2.2999999999999994</v>
+      </c>
+      <c r="Q17">
+        <f>SUM(Q2:Q16)</f>
+        <v>-9.0500000000000007</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q20">
-    <sortCondition descending="1" ref="Q1:Q20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Q16">
+    <sortCondition descending="1" ref="Q1:Q16"/>
   </sortState>
-  <conditionalFormatting sqref="B1:P1">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A2:A16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -2086,7 +2168,678 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B1:P1">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2:P16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{217596E7-7356-454A-9117-803D03CC9867}">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.05</v>
+      </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.15</v>
+      </c>
+      <c r="Q2">
+        <f>SUM(B2:P2)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>-0.3</v>
+      </c>
+      <c r="N3">
+        <v>0.15</v>
+      </c>
+      <c r="Q3">
+        <f>SUM(B3:P3)</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0.15</v>
+      </c>
+      <c r="M4">
+        <v>-0.3</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <f>SUM(B4:P4)</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.15</v>
+      </c>
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>0.15</v>
+      </c>
+      <c r="E5">
+        <v>-0.3</v>
+      </c>
+      <c r="F5">
+        <v>-0.3</v>
+      </c>
+      <c r="G5">
+        <v>-0.15</v>
+      </c>
+      <c r="J5">
+        <v>-0.3</v>
+      </c>
+      <c r="K5">
+        <v>-0.3</v>
+      </c>
+      <c r="L5">
+        <v>0.05</v>
+      </c>
+      <c r="O5">
+        <v>-0.15</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <f>SUM(B5:P5)</f>
+        <v>-9.9999999999999867E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.15</v>
+      </c>
+      <c r="D6">
+        <v>0.05</v>
+      </c>
+      <c r="E6">
+        <v>-0.3</v>
+      </c>
+      <c r="F6">
+        <v>-0.3</v>
+      </c>
+      <c r="G6">
+        <v>-0.15</v>
+      </c>
+      <c r="I6">
+        <v>-0.3</v>
+      </c>
+      <c r="J6">
+        <v>-0.3</v>
+      </c>
+      <c r="K6">
+        <v>0.15</v>
+      </c>
+      <c r="L6">
+        <v>0.05</v>
+      </c>
+      <c r="M6">
+        <v>-0.3</v>
+      </c>
+      <c r="O6">
+        <v>-0.15</v>
+      </c>
+      <c r="P6">
+        <v>0.15</v>
+      </c>
+      <c r="Q6">
+        <f>SUM(B6:P6)</f>
+        <v>-0.25000000000000011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>-0.15</v>
+      </c>
+      <c r="C7">
+        <v>-0.3</v>
+      </c>
+      <c r="D7">
+        <v>-0.3</v>
+      </c>
+      <c r="E7">
+        <v>0.05</v>
+      </c>
+      <c r="G7">
+        <v>0.15</v>
+      </c>
+      <c r="I7">
+        <v>-0.3</v>
+      </c>
+      <c r="K7">
+        <v>-0.15</v>
+      </c>
+      <c r="L7">
+        <v>-0.3</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>-0.15</v>
+      </c>
+      <c r="Q7">
+        <f>SUM(B7:P7)</f>
+        <v>-0.44999999999999984</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.15</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.05</v>
+      </c>
+      <c r="E8">
+        <v>-0.15</v>
+      </c>
+      <c r="F8">
+        <v>-0.3</v>
+      </c>
+      <c r="G8">
+        <v>-0.3</v>
+      </c>
+      <c r="I8">
+        <v>-0.3</v>
+      </c>
+      <c r="J8">
+        <v>-0.3</v>
+      </c>
+      <c r="K8">
+        <v>0.05</v>
+      </c>
+      <c r="L8">
+        <v>0.15</v>
+      </c>
+      <c r="M8">
+        <v>-0.3</v>
+      </c>
+      <c r="O8">
+        <v>-0.3</v>
+      </c>
+      <c r="P8">
+        <v>0.05</v>
+      </c>
+      <c r="Q8">
+        <f>SUM(B8:P8)</f>
+        <v>-0.49999999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>-0.15</v>
+      </c>
+      <c r="C9">
+        <v>-0.3</v>
+      </c>
+      <c r="E9">
+        <v>0.15</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>-0.3</v>
+      </c>
+      <c r="J9">
+        <v>-0.3</v>
+      </c>
+      <c r="K9">
+        <v>-0.15</v>
+      </c>
+      <c r="L9">
+        <v>-0.3</v>
+      </c>
+      <c r="M9">
+        <v>-0.3</v>
+      </c>
+      <c r="O9">
+        <v>0.15</v>
+      </c>
+      <c r="P9">
+        <v>-0.15</v>
+      </c>
+      <c r="Q9">
+        <f>SUM(B9:P9)</f>
+        <v>-0.64999999999999991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0.05</v>
+      </c>
+      <c r="C10">
+        <v>0.15</v>
+      </c>
+      <c r="E10">
+        <v>-0.15</v>
+      </c>
+      <c r="F10">
+        <v>-0.3</v>
+      </c>
+      <c r="G10">
+        <v>-0.3</v>
+      </c>
+      <c r="I10">
+        <v>-0.3</v>
+      </c>
+      <c r="J10">
+        <v>-0.3</v>
+      </c>
+      <c r="K10">
+        <v>-0.3</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>-0.3</v>
+      </c>
+      <c r="P10">
+        <v>0.05</v>
+      </c>
+      <c r="Q10">
+        <f>SUM(B10:P10)</f>
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>0.15</v>
+      </c>
+      <c r="C11">
+        <v>0.05</v>
+      </c>
+      <c r="E11">
+        <v>-0.3</v>
+      </c>
+      <c r="F11">
+        <v>-0.3</v>
+      </c>
+      <c r="G11">
+        <v>-0.15</v>
+      </c>
+      <c r="I11">
+        <v>-0.3</v>
+      </c>
+      <c r="J11">
+        <v>-0.3</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>-0.3</v>
+      </c>
+      <c r="O11">
+        <v>-0.15</v>
+      </c>
+      <c r="P11">
+        <v>-0.3</v>
+      </c>
+      <c r="Q11">
+        <f>SUM(B11:P11)</f>
+        <v>-0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>-0.3</v>
+      </c>
+      <c r="C12">
+        <v>-0.15</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>-0.3</v>
+      </c>
+      <c r="G12">
+        <v>0.15</v>
+      </c>
+      <c r="I12">
+        <v>-0.3</v>
+      </c>
+      <c r="J12">
+        <v>-0.3</v>
+      </c>
+      <c r="K12">
+        <v>-0.3</v>
+      </c>
+      <c r="L12">
+        <v>-0.15</v>
+      </c>
+      <c r="M12">
+        <v>-0.3</v>
+      </c>
+      <c r="O12">
+        <v>0.05</v>
+      </c>
+      <c r="P12">
+        <v>-0.3</v>
+      </c>
+      <c r="Q12">
+        <f>SUM(B12:P12)</f>
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>-0.3</v>
+      </c>
+      <c r="C13">
+        <v>-0.3</v>
+      </c>
+      <c r="D13">
+        <v>-0.3</v>
+      </c>
+      <c r="E13">
+        <v>-0.3</v>
+      </c>
+      <c r="F13">
+        <v>0.15</v>
+      </c>
+      <c r="G13">
+        <v>-0.3</v>
+      </c>
+      <c r="I13">
+        <v>-0.3</v>
+      </c>
+      <c r="J13">
+        <v>-0.3</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>-0.3</v>
+      </c>
+      <c r="Q13">
+        <f>SUM(B13:P13)</f>
+        <v>-1.2500000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>-0.3</v>
+      </c>
+      <c r="C14">
+        <v>-0.3</v>
+      </c>
+      <c r="D14">
+        <v>-0.3</v>
+      </c>
+      <c r="E14">
+        <v>-0.3</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>-0.3</v>
+      </c>
+      <c r="J14">
+        <v>-0.3</v>
+      </c>
+      <c r="K14">
+        <v>-0.3</v>
+      </c>
+      <c r="L14">
+        <v>-0.3</v>
+      </c>
+      <c r="M14">
+        <v>0.15</v>
+      </c>
+      <c r="P14">
+        <v>-0.3</v>
+      </c>
+      <c r="Q14">
+        <f>SUM(B14:P14)</f>
+        <v>-1.55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>-0.3</v>
+      </c>
+      <c r="C15">
+        <v>-0.3</v>
+      </c>
+      <c r="E15">
+        <v>-0.3</v>
+      </c>
+      <c r="F15">
+        <v>-0.3</v>
+      </c>
+      <c r="G15">
+        <v>-0.3</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>-0.3</v>
+      </c>
+      <c r="K15">
+        <v>-0.3</v>
+      </c>
+      <c r="L15">
+        <v>-0.3</v>
+      </c>
+      <c r="M15">
+        <v>-0.3</v>
+      </c>
+      <c r="O15">
+        <v>-0.3</v>
+      </c>
+      <c r="Q15">
+        <f>SUM(B15:P15)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>-0.3</v>
+      </c>
+      <c r="C16">
+        <v>-0.3</v>
+      </c>
+      <c r="D16">
+        <v>-0.15</v>
+      </c>
+      <c r="E16">
+        <v>-0.3</v>
+      </c>
+      <c r="F16">
+        <v>-0.3</v>
+      </c>
+      <c r="G16">
+        <v>-0.3</v>
+      </c>
+      <c r="H16">
+        <v>-0.3</v>
+      </c>
+      <c r="I16">
+        <v>-0.3</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>-0.3</v>
+      </c>
+      <c r="L16">
+        <v>-0.3</v>
+      </c>
+      <c r="M16">
+        <v>-0.3</v>
+      </c>
+      <c r="P16">
+        <v>-0.3</v>
+      </c>
+      <c r="Q16">
+        <f>SUM(B16:P16)</f>
+        <v>-2.4499999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <f>SUM(Q2:Q16)</f>
+        <v>-9.0499999999999989</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q16">
+    <sortCondition descending="1" ref="Q1:Q16"/>
+  </sortState>
+  <conditionalFormatting sqref="A1:P16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
fix table error, fix algorithm
</commit_message>
<xml_diff>
--- a/relationship.xlsx
+++ b/relationship.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mark\Documents\Mark\Project\20210606 Dynamic Relationship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3409CD98-D620-49A5-B573-776CF4F546BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E4E11DB1-D0E4-4206-ADEE-B96A33E08F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C0A86CE9-5774-486B-821C-E24FED4D1238}"/>
+    <workbookView xWindow="2415" yWindow="2280" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{C0A86CE9-5774-486B-821C-E24FED4D1238}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
   <si>
     <t>Terran</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>TerraCorp</t>
+  </si>
+  <si>
+    <t>passive gain</t>
+  </si>
+  <si>
+    <t>active gain</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1230,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,6 +1281,9 @@
       <c r="P1" t="s">
         <v>12</v>
       </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1380,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <f>SUM(B3:P3)</f>
+        <f t="shared" ref="Q3:Q16" si="0">SUM(B3:P3)</f>
         <v>0.84999999999999987</v>
       </c>
     </row>
@@ -1401,10 +1410,10 @@
         <v>0.15</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="G4">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H4">
         <v>0.05</v>
@@ -1419,23 +1428,23 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="Q4">
-        <f>SUM(B4:P4)</f>
-        <v>1.25</v>
+        <f t="shared" si="0"/>
+        <v>0.24999999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1488,7 +1497,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q5">
-        <f>SUM(B5:P5)</f>
+        <f t="shared" si="0"/>
         <v>-9.9999999999999978E-2</v>
       </c>
     </row>
@@ -1503,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>-0.15</v>
@@ -1542,8 +1551,8 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <f>SUM(B6:P6)</f>
-        <v>-0.44999999999999996</v>
+        <f t="shared" si="0"/>
+        <v>-0.15000000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1557,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E7">
         <v>0.15</v>
@@ -1596,8 +1605,8 @@
         <v>-0.3</v>
       </c>
       <c r="Q7">
-        <f>SUM(B7:P7)</f>
-        <v>-0.25000000000000006</v>
+        <f t="shared" si="0"/>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1650,7 +1659,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q8">
-        <f>SUM(B8:P8)</f>
+        <f t="shared" si="0"/>
         <v>-0.49999999999999994</v>
       </c>
     </row>
@@ -1704,7 +1713,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q9">
-        <f>SUM(B9:P9)</f>
+        <f t="shared" si="0"/>
         <v>-0.64999999999999991</v>
       </c>
     </row>
@@ -1758,7 +1767,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q10">
-        <f>SUM(B10:P10)</f>
+        <f t="shared" si="0"/>
         <v>-0.7</v>
       </c>
     </row>
@@ -1812,7 +1821,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q11">
-        <f>SUM(B11:P11)</f>
+        <f t="shared" si="0"/>
         <v>-0.89999999999999991</v>
       </c>
     </row>
@@ -1827,7 +1836,7 @@
         <v>-0.3</v>
       </c>
       <c r="D12">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1866,8 +1875,8 @@
         <v>-0.3</v>
       </c>
       <c r="Q12">
-        <f>SUM(B12:P12)</f>
-        <v>-1.25</v>
+        <f t="shared" si="0"/>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1920,7 +1929,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q13">
-        <f>SUM(B13:P13)</f>
+        <f t="shared" si="0"/>
         <v>-1.2000000000000002</v>
       </c>
     </row>
@@ -1935,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>-0.3</v>
@@ -1974,8 +1983,8 @@
         <v>-0.3</v>
       </c>
       <c r="Q14">
-        <f>SUM(B14:P14)</f>
-        <v>-1.5500000000000003</v>
+        <f t="shared" si="0"/>
+        <v>-1.2500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -2028,7 +2037,7 @@
         <v>-0.3</v>
       </c>
       <c r="Q15">
-        <f>SUM(B15:P15)</f>
+        <f t="shared" si="0"/>
         <v>-1.9999999999999998</v>
       </c>
     </row>
@@ -2043,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>-0.3</v>
@@ -2082,82 +2091,85 @@
         <v>1</v>
       </c>
       <c r="Q16">
-        <f>SUM(B16:P16)</f>
-        <v>-2.4499999999999993</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f>SUM(B2:B16)</f>
-        <v>0.84999999999999987</v>
-      </c>
-      <c r="C17">
-        <f t="shared" ref="C17:P17" si="0">SUM(C2:C16)</f>
-        <v>0.84999999999999987</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0.19999999999999993</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>-9.9999999999999978E-2</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>-0.15000000000000002</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>-0.25000000000000006</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>-0.49999999999999994</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>-0.64999999999999991</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>-0.7</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>-0.89999999999999991</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
-        <v>-0.95</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="0"/>
-        <v>-1.2000000000000002</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="0"/>
-        <v>-1.2500000000000002</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="0"/>
-        <v>-1.9999999999999998</v>
-      </c>
-      <c r="P17">
         <f t="shared" si="0"/>
         <v>-2.2999999999999994</v>
       </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:O17" si="1">SUM(B2:B16)</f>
+        <v>0.84999999999999987</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.84999999999999987</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>-9.9999999999999978E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>-0.44999999999999996</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>-0.2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>-0.49999999999999994</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>-0.64999999999999991</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>-0.7</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>-1.25</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>-1.2000000000000002</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>-1.5500000000000003</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>-1.9999999999999998</v>
+      </c>
+      <c r="P17">
+        <f>SUM(P2:P16)</f>
+        <v>-2.4499999999999993</v>
+      </c>
       <c r="Q17">
         <f>SUM(Q2:Q16)</f>
-        <v>-9.0500000000000007</v>
+        <v>-8.9499999999999993</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Q16">
     <sortCondition descending="1" ref="Q1:Q16"/>
   </sortState>
-  <conditionalFormatting sqref="A2:A16">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="A2:A17">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2168,8 +2180,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:P1">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="B1:Q1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2181,7 +2193,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:P16">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>